<commit_message>
Added new feature to calculate variables by specifying desired build area versus extrusion lengths.
</commit_message>
<xml_diff>
--- a/kossel_frame_calc.xlsx
+++ b/kossel_frame_calc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="16275" windowHeight="9780"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="16275" windowHeight="9720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>mm length of horizontal OpenBeam (triangle)</t>
   </si>
@@ -205,6 +205,27 @@
   </si>
   <si>
     <t>Enter your build parameters in these inputs</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>DELTA_RADIUS/ Horizontal radius</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: Diagonal Rod Horizontal length </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -685,7 +706,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,13 +734,13 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D2">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="E2" t="s">
         <v>26</v>
@@ -733,7 +754,7 @@
         <v>23</v>
       </c>
       <c r="D3">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="E3" t="s">
         <v>27</v>
@@ -766,7 +787,7 @@
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
-        <v>28</v>
+        <v>21.1</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>6</v>
@@ -800,14 +821,14 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <f>A12-A6-A5</f>
-        <v>104.55444566227678</v>
+        <v>112.63734943093152</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="17">
         <f>D2*SQRT(2)</f>
-        <v>197.98989873223331</v>
+        <v>176.77669529663689</v>
       </c>
       <c r="E11" t="s">
         <v>20</v>
@@ -816,14 +837,14 @@
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f>(A18/2)/SIN(60*PI()/180 )</f>
-        <v>151.55444566227678</v>
+        <v>159.63734943093152</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="2">
         <f>D11/2</f>
-        <v>98.994949366116657</v>
+        <v>88.388347648318444</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>18</v>
@@ -832,14 +853,14 @@
     <row r="13" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <f>((A11*2)-A5)/COS(A7*PI()/180)</f>
-        <v>214.17906663319761</v>
+        <v>220.02671215588472</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="2">
         <f>(D12+A4/2+4-A5)/SIN(PI()/6)</f>
-        <v>180.98989873223334</v>
+        <v>159.77669529663692</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>10</v>
@@ -848,30 +869,30 @@
     <row r="14" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <f>SQRT((A13*A13)-(A11*A11))</f>
-        <v>186.92522696554821</v>
+        <v>189.00947482944548</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="16">
         <f>D13-A6-A5</f>
-        <v>133.98989873223334</v>
+        <v>112.77669529663692</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <f>ACOS(A11/A13)*180/PI()</f>
-        <v>60.780041789092891</v>
+        <v>59.207808706668516</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="14">
         <f>(D13*SIN(PI()/3)-11.25)*2</f>
-        <v>290.98370026097405</v>
+        <v>254.2413541192264</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>0</v>
@@ -880,21 +901,21 @@
     <row r="16" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15">
         <f>A12*SIN(PI()/6)+A5-A4/2-4</f>
-        <v>84.277222831138374</v>
+        <v>88.318674715465747</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="16">
         <f>((D14*2)-A5)/COS(A7*PI()/180)</f>
-        <v>280.85449178418867</v>
+        <v>220.32543199669965</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F16">
         <f>D16/25.4</f>
-        <v>11.057263456070421</v>
+        <v>8.6742296061692787</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -904,7 +925,7 @@
       </c>
       <c r="D17" s="2">
         <f>ACOS(D14/D16)*180/PI()</f>
-        <v>61.505172419059221</v>
+        <v>59.211918587353416</v>
       </c>
       <c r="E17" s="10" t="s">
         <v>21</v>
@@ -913,14 +934,14 @@
     <row r="18" spans="1:5" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <f>A2+22.5</f>
-        <v>262.5</v>
+        <v>276.5</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="2">
         <f>SQRT((D16*D16)-(D14*D14))</f>
-        <v>246.83183059135777</v>
+        <v>189.27417410334098</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>12</v>
@@ -929,14 +950,14 @@
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <f>A16*2</f>
-        <v>168.55444566227675</v>
+        <v>176.63734943093149</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="14">
         <f>D3+A14+A21+A8</f>
-        <v>568.92522696554818</v>
+        <v>548.00947482944548</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>22</v>
@@ -945,7 +966,7 @@
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <f>A19/SQRT(2)</f>
-        <v>119.18599152693533</v>
+        <v>124.9014675934294</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>2</v>
@@ -963,7 +984,7 @@
     <row r="22" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <f>A3-A14-A21-A8</f>
-        <v>231.07477303445182</v>
+        <v>228.99052517055452</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>16</v>

</xml_diff>